<commit_message>
roteiro de bd atualizado
</commit_message>
<xml_diff>
--- a/sprint-1-bd/apoio/exemplo-01.xlsx
+++ b/sprint-1-bd/apoio/exemplo-01.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5436C801-F715-425C-844E-EB7815191843}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cursos-1" sheetId="1" r:id="rId1"/>
@@ -12,6 +13,8 @@
     <sheet name="cursos-3" sheetId="3" r:id="rId3"/>
     <sheet name="cursos-4" sheetId="4" r:id="rId4"/>
     <sheet name="cursos-5" sheetId="5" r:id="rId5"/>
+    <sheet name="cursos-6" sheetId="7" r:id="rId6"/>
+    <sheet name="cursos-7" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="14">
-  <si>
-    <t>Matérias</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="19">
   <si>
     <t>Nome</t>
   </si>
@@ -66,11 +66,29 @@
   <si>
     <t>Lógico</t>
   </si>
+  <si>
+    <t>Alunos</t>
+  </si>
+  <si>
+    <t>IdAluno</t>
+  </si>
+  <si>
+    <t>Tadeu</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>CursosAlunos</t>
+  </si>
+  <si>
+    <t>Disciplinas</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -181,7 +199,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Conector de Seta Reta 2"/>
+        <xdr:cNvPr id="3" name="Conector de Seta Reta 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -228,7 +252,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="6" name="Conector Angulado 5"/>
+        <xdr:cNvPr id="6" name="Conector Angulado 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -275,7 +305,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Imagem 9"/>
+        <xdr:cNvPr id="10" name="Imagem 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -319,7 +355,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Imagem 10"/>
+        <xdr:cNvPr id="11" name="Imagem 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -340,6 +382,695 @@
         <a:xfrm>
           <a:off x="0" y="3731559"/>
           <a:ext cx="4200525" cy="904875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>93636</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3228</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="Conector de Seta Reta 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38A55B57-B0D1-42D8-B52C-0B6A7A926509}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2819400" y="474636"/>
+          <a:ext cx="1222428" cy="1615"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>90488</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2381</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>87179</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Conector Angulado 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20257736-B6F1-4817-93FA-FD2074B35E8F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2819400" y="661988"/>
+          <a:ext cx="1221581" cy="377691"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>3922</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagem 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFE78E61-8456-4C7E-9D0F-3854791546E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1994647"/>
+          <a:ext cx="6677025" cy="3533775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>166407</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagem 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D380FDC6-FA88-4F0E-AF6E-B7719F437F73}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="6286500"/>
+          <a:ext cx="4200525" cy="2571750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>33620</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>156886</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>313765</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Conector: Angulado 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB219763-1B4B-4488-94BA-728ECC888CAB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="6096002" y="537886"/>
+          <a:ext cx="3227292" cy="268938"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 67361"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>93636</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3228</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="Conector de Seta Reta 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77FFC356-35D1-4EC3-AA12-F58EE6483EE5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2819400" y="474636"/>
+          <a:ext cx="1222428" cy="1615"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>90488</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2381</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>87179</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Conector Angulado 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{482CA78E-4A7A-4E7F-A872-2F04D22C45A1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2819400" y="661988"/>
+          <a:ext cx="1221581" cy="377691"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>11206</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>593912</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Conector de Seta Reta 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBB78793-B017-416F-A6E2-78771F0FF0FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="9020735" y="470647"/>
+          <a:ext cx="582706" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>85165</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>600635</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>91109</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Conector de Seta Reta 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D015400-9409-4315-85E9-326DCEA7210C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6062870" y="466165"/>
+          <a:ext cx="1213548" cy="5944"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>488</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>96371</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>601123</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>102315</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Conector de Seta Reta 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36D60058-411D-4174-8086-5AC9AF1348FF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6062870" y="667871"/>
+          <a:ext cx="1205753" cy="5944"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>33618</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>100853</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>582706</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>112059</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Conector: Angulado 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4519A702-3E94-45AC-979D-EECD7B4BE0ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="9043147" y="481853"/>
+          <a:ext cx="549088" cy="201706"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>112059</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>166407</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>16809</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Imagem 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F73D823-D2F4-4199-A36A-76ADBC13D5F1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="6017559"/>
+          <a:ext cx="4200525" cy="2571750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>134470</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>48745</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Imagem 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64D1D2D7-B33B-400A-9B2E-6BE830EE8EC0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1848970"/>
+          <a:ext cx="6677025" cy="3533775"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -613,11 +1344,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,27 +1358,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -656,11 +1387,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A6"/>
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,32 +1401,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -704,11 +1435,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:B6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,16 +1450,16 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -736,7 +1467,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -744,7 +1475,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -752,7 +1483,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -760,7 +1491,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -772,11 +1503,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:C6"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,20 +1519,20 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -809,10 +1540,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -820,10 +1551,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -831,10 +1562,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -842,10 +1573,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -857,11 +1588,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,30 +1606,30 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="F1" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -906,7 +1637,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
@@ -915,7 +1646,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -923,7 +1654,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
@@ -932,7 +1663,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -940,7 +1671,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
@@ -951,7 +1682,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="2">
         <v>2</v>
@@ -959,12 +1690,12 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -975,4 +1706,329 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AA1346B-D54D-4458-B74E-E28099FF572D}">
+  <dimension ref="A1:L32"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="F1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="4"/>
+      <c r="J1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="2">
+        <v>1</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="2">
+        <v>2</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="J1:L1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6B10D12-1D16-45BF-90EE-C1435496BDDD}">
+  <dimension ref="A1:N31"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P35" sqref="P35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="F1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="4"/>
+      <c r="J1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="4"/>
+      <c r="M1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="4"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="2">
+        <v>1</v>
+      </c>
+      <c r="K3" s="2">
+        <v>1</v>
+      </c>
+      <c r="M3" s="2">
+        <v>1</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="2">
+        <v>2</v>
+      </c>
+      <c r="K4" s="2">
+        <v>1</v>
+      </c>
+      <c r="M4" s="2">
+        <v>2</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="J1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>